<commit_message>
Shift Changed to DEPT name
made changes to name the shift similar to department name.
</commit_message>
<xml_diff>
--- a/media/shopConfig.xlsx
+++ b/media/shopConfig.xlsx
@@ -12,7 +12,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+  <si>
+    <t>employeeName</t>
+  </si>
   <si>
     <t>date</t>
   </si>
@@ -20,9 +23,6 @@
     <t>shiftStartTime</t>
   </si>
   <si>
-    <t>employeeName</t>
-  </si>
-  <si>
     <t>shiftEndTime</t>
   </si>
   <si>
@@ -35,6 +35,27 @@
     <t>2016-11-22</t>
   </si>
   <si>
+    <t>shift1</t>
+  </si>
+  <si>
+    <t>shope opened late</t>
+  </si>
+  <si>
+    <t>2016-11-23</t>
+  </si>
+  <si>
+    <t>holiday</t>
+  </si>
+  <si>
+    <t>business holiday</t>
+  </si>
+  <si>
+    <t>shift2</t>
+  </si>
+  <si>
+    <t>2016-11-26</t>
+  </si>
+  <si>
     <t>shift</t>
   </si>
   <si>
@@ -44,7 +65,7 @@
     <t>prem</t>
   </si>
   <si>
-    <t>shift1</t>
+    <t>DEPT1</t>
   </si>
   <si>
     <t>vipin</t>
@@ -59,36 +80,21 @@
     <t>ritesh</t>
   </si>
   <si>
-    <t>shift2</t>
-  </si>
-  <si>
     <t>naveen</t>
   </si>
   <si>
     <t>mainank</t>
   </si>
   <si>
-    <t>shope opened late</t>
-  </si>
-  <si>
     <t>nandan</t>
   </si>
   <si>
-    <t>2016-11-23</t>
-  </si>
-  <si>
     <t>sonu</t>
   </si>
   <si>
-    <t>holiday</t>
-  </si>
-  <si>
     <t>mannu</t>
   </si>
   <si>
-    <t>business holiday</t>
-  </si>
-  <si>
     <t>neeraj</t>
   </si>
   <si>
@@ -110,9 +116,6 @@
     <t>rajnee</t>
   </si>
   <si>
-    <t>2016-11-26</t>
-  </si>
-  <si>
     <t>sheetal</t>
   </si>
   <si>
@@ -120,6 +123,9 @@
   </si>
   <si>
     <t>pooja</t>
+  </si>
+  <si>
+    <t>DEPT2</t>
   </si>
   <si>
     <t>balwant</t>
@@ -141,7 +147,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -152,6 +158,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -167,18 +174,24 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="21" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -212,24 +225,24 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3">
@@ -238,16 +251,16 @@
       <c r="C2" s="3">
         <v>0.8541666666666666</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>20</v>
+      <c r="A3" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>0.4166666666666667</v>
@@ -255,15 +268,15 @@
       <c r="C3" s="3">
         <v>0.8333333333333334</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="3">
@@ -272,16 +285,16 @@
       <c r="C4" s="3">
         <v>0.8541666666666666</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>32</v>
+      <c r="A5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>0.4166666666666667</v>
@@ -289,15 +302,15 @@
       <c r="C5" s="3">
         <v>0.8333333333333334</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>24</v>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3">
@@ -306,11 +319,11 @@
       <c r="C6" s="3">
         <v>0.8333333333333334</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>24</v>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1"/>
@@ -1327,22 +1340,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C2">
         <v>10000.0</v>
@@ -1350,10 +1363,10 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
+        <v>18</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C3">
         <v>30000.0</v>
@@ -1361,10 +1374,10 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
+        <v>19</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C4">
         <v>30000.0</v>
@@ -1372,10 +1385,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C5">
         <v>30000.0</v>
@@ -1383,10 +1396,10 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C6">
         <v>40000.0</v>
@@ -1394,10 +1407,10 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C7">
         <v>40000.0</v>
@@ -1405,10 +1418,10 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
       </c>
       <c r="C8">
         <v>40000.0</v>
@@ -1416,10 +1429,10 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C9">
         <v>40000.0</v>
@@ -1427,10 +1440,10 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
+        <v>25</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C10">
         <v>40000.0</v>
@@ -1438,10 +1451,10 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C11">
         <v>40000.0</v>
@@ -1449,10 +1462,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
+        <v>27</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C12">
         <v>40000.0</v>
@@ -1460,10 +1473,10 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C13">
         <v>40000.0</v>
@@ -1471,10 +1484,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
+        <v>29</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C14">
         <v>40000.0</v>
@@ -1482,10 +1495,10 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C15">
         <v>40000.0</v>
@@ -1493,10 +1506,10 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C16">
         <v>40000.0</v>
@@ -1504,10 +1517,10 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
+        <v>32</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C17">
         <v>40000.0</v>
@@ -1515,10 +1528,10 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
+        <v>33</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C18">
         <v>40000.0</v>
@@ -1526,10 +1539,10 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
+        <v>34</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C19">
         <v>40000.0</v>
@@ -1537,10 +1550,10 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C20">
         <v>40000.0</v>
@@ -1548,10 +1561,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
+        <v>36</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C21">
         <v>40000.0</v>
@@ -1559,10 +1572,10 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
+        <v>38</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C22">
         <v>40000.0</v>
@@ -1570,10 +1583,10 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>10</v>
       </c>
       <c r="C23">
         <v>40000.0</v>
@@ -1581,10 +1594,10 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
+        <v>40</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C24">
         <v>40000.0</v>
@@ -1592,10 +1605,10 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C25">
         <v>40000.0</v>
@@ -1603,10 +1616,10 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
-        <v>10</v>
+        <v>42</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C26">
         <v>40000.0</v>

</xml_diff>